<commit_message>
API Automation 22nd Jan latest
</commit_message>
<xml_diff>
--- a/src/test/resources/data/PublishingSubsidiesAPIDatasheet.xlsx
+++ b/src/test/resources/data/PublishingSubsidiesAPIDatasheet.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1403" uniqueCount="349">
   <si>
     <t>Training</t>
   </si>
@@ -1058,6 +1058,12 @@
   </si>
   <si>
     <t>Subsidy Element Full Amount is mandatory.|Subsidy Element Full Amount is invalid.</t>
+  </si>
+  <si>
+    <t>Subsidy Element Full Amount Range is mandatory when Subsidy Instrument is Tax Measure.</t>
+  </si>
+  <si>
+    <t>Subsidy Control number does not exists.</t>
   </si>
   <si>
     <r>
@@ -1066,12 +1072,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Subsidy Measure Title must be 255 characters or fewer </t>
+      <t>Subsidy Measure Title must be 255 characters or fewer</t>
     </r>
     <r>
       <rPr>
@@ -1086,12 +1091,11 @@
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Size of Organization  field is mandatory.</t>
+      <t>Size of Organization field is mandatory.</t>
     </r>
     <r>
       <rPr>
@@ -1101,17 +1105,16 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>|Size of Organization  field is mandatory.|Spending Region field is mandatory.|Spending Region field is mandatory.|Spending Sector field is mandatory.|Spending Sector field is mandatory.|Goods or Services field is mandatory.|Goods or Services field is mandatory.|</t>
+      <t>|Size of Organization field is mandatory.|Spending Region field is mandatory.|Spending Region field is mandatory.|Spending Sector field is mandatory.|Spending Sector field is mandatory.|Goods or Services field is mandatory.|Goods or Services field is mandatory.|</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <color rgb="FFFF0000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Subsidy Element Full Amount Range is mandatory when Subsidy Instrument is Tax Measure .</t>
+      <t>Subsidy Element Full Amount Range is mandatory when Subsidy Instrument is Tax Measure.</t>
     </r>
     <r>
       <rPr>
@@ -1125,10 +1128,7 @@
     </r>
   </si>
   <si>
-    <t>Subsidy Control Number does not exists.</t>
-  </si>
-  <si>
-    <t>Subsidy Element Full Amount Range is mandatory when Subsidy Instrument is Tax Measure.</t>
+    <t>StatusCode</t>
   </si>
 </sst>
 </file>
@@ -1164,7 +1164,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1179,7 +1178,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1222,7 +1221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1261,20 +1260,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1567,11 +1563,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V86"/>
+  <dimension ref="A1:W86"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="U37" sqref="U37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1589,9 +1585,10 @@
     <col min="20" max="20" width="25.7265625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="63.7265625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="25.54296875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1658,8 +1655,11 @@
       <c r="V1" s="3" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W1" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>166</v>
       </c>
@@ -1718,8 +1718,11 @@
       <c r="V2" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W2" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>167</v>
       </c>
@@ -1782,8 +1785,11 @@
       <c r="V3" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="4" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W3" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>168</v>
       </c>
@@ -1842,8 +1848,11 @@
       <c r="V4" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="5" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W4" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A5" s="5" t="s">
         <v>169</v>
       </c>
@@ -1902,8 +1911,11 @@
       <c r="V5" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="6" spans="1:22" ht="56" x14ac:dyDescent="0.35">
+      <c r="W5" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>170</v>
       </c>
@@ -1962,8 +1974,11 @@
       <c r="V6" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W6" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7" s="5" t="s">
         <v>171</v>
       </c>
@@ -1976,7 +1991,7 @@
       <c r="D7" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="14">
         <v>10323184</v>
       </c>
       <c r="F7" s="11" t="s">
@@ -2022,8 +2037,11 @@
       <c r="V7" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W7" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A8" s="5" t="s">
         <v>172</v>
       </c>
@@ -2082,8 +2100,11 @@
       <c r="V8" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W8" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
         <v>173</v>
       </c>
@@ -2142,8 +2163,11 @@
       <c r="V9" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W9" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A10" s="5" t="s">
         <v>174</v>
       </c>
@@ -2202,8 +2226,11 @@
       <c r="V10" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W10" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>175</v>
       </c>
@@ -2216,7 +2243,7 @@
       <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="15">
+      <c r="E11" s="14">
         <v>1378312</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -2262,8 +2289,11 @@
       <c r="V11" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W11" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>176</v>
       </c>
@@ -2322,8 +2352,11 @@
       <c r="V12" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W12" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A13" s="5" t="s">
         <v>177</v>
       </c>
@@ -2382,8 +2415,11 @@
       <c r="V13" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="14" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W13" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A14" s="5" t="s">
         <v>178</v>
       </c>
@@ -2442,8 +2478,11 @@
       <c r="V14" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="15" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W14" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A15" s="5" t="s">
         <v>179</v>
       </c>
@@ -2456,7 +2495,7 @@
       <c r="D15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="14">
         <v>2021215</v>
       </c>
       <c r="F15" s="11" t="s">
@@ -2502,8 +2541,11 @@
       <c r="V15" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W15" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A16" s="5" t="s">
         <v>180</v>
       </c>
@@ -2562,8 +2604,11 @@
       <c r="V16" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W16" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A17" s="5" t="s">
         <v>181</v>
       </c>
@@ -2622,8 +2667,11 @@
       <c r="V17" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W17" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A18" s="5" t="s">
         <v>182</v>
       </c>
@@ -2682,8 +2730,11 @@
       <c r="V18" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W18" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A19" s="5" t="s">
         <v>183</v>
       </c>
@@ -2742,8 +2793,11 @@
       <c r="V19" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W19" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>184</v>
       </c>
@@ -2802,8 +2856,11 @@
       <c r="V20" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W20" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>185</v>
       </c>
@@ -2862,8 +2919,11 @@
       <c r="V21" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W21" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A22" s="5" t="s">
         <v>186</v>
       </c>
@@ -2922,8 +2982,11 @@
       <c r="V22" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="42" x14ac:dyDescent="0.35">
+      <c r="W22" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
         <v>187</v>
       </c>
@@ -2982,8 +3045,11 @@
       <c r="V23" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W23" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A24" s="5" t="s">
         <v>188</v>
       </c>
@@ -3042,8 +3108,11 @@
       <c r="V24" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W24" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>189</v>
       </c>
@@ -3102,8 +3171,11 @@
       <c r="V25" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W25" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A26" s="5" t="s">
         <v>190</v>
       </c>
@@ -3162,8 +3234,11 @@
       <c r="V26" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W26" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A27" s="5" t="s">
         <v>225</v>
       </c>
@@ -3172,7 +3247,7 @@
       <c r="D27" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E27" s="10">
+      <c r="E27" s="14">
         <v>100002389</v>
       </c>
       <c r="F27" s="11" t="s">
@@ -3222,8 +3297,11 @@
       <c r="V27" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="28" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W27" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A28" s="5" t="s">
         <v>226</v>
       </c>
@@ -3236,7 +3314,7 @@
       <c r="D28" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="10">
+      <c r="E28" s="14">
         <v>58614000</v>
       </c>
       <c r="F28" s="11" t="s">
@@ -3290,8 +3368,11 @@
       <c r="V28" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="29" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W28" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A29" s="5" t="s">
         <v>227</v>
       </c>
@@ -3304,7 +3385,7 @@
       <c r="D29" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="14">
         <v>58614000</v>
       </c>
       <c r="F29" s="11" t="s">
@@ -3348,14 +3429,17 @@
       <c r="T29" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="U29" s="17" t="s">
+      <c r="U29" s="16" t="s">
         <v>346</v>
       </c>
       <c r="V29" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="30" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W29" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
         <v>228</v>
       </c>
@@ -3368,7 +3452,7 @@
       <c r="D30" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="14">
         <v>100002389</v>
       </c>
       <c r="F30" s="11" t="s">
@@ -3412,14 +3496,17 @@
       <c r="T30" s="13" t="s">
         <v>304</v>
       </c>
-      <c r="U30" s="17" t="s">
+      <c r="U30" s="16" t="s">
         <v>346</v>
       </c>
       <c r="V30" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="31" spans="1:22" ht="126" x14ac:dyDescent="0.35">
+      <c r="W30" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" ht="126" x14ac:dyDescent="0.35">
       <c r="A31" s="5" t="s">
         <v>229</v>
       </c>
@@ -3432,7 +3519,7 @@
       <c r="D31" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E31" s="10">
+      <c r="E31" s="14">
         <v>58614000</v>
       </c>
       <c r="F31" s="11" t="s">
@@ -3477,7 +3564,7 @@
       <c r="S31" s="13">
         <v>2</v>
       </c>
-      <c r="T31" s="18" t="s">
+      <c r="T31" s="16" t="s">
         <v>337</v>
       </c>
       <c r="U31" s="13" t="s">
@@ -3486,8 +3573,11 @@
       <c r="V31" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="32" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W31" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>230</v>
       </c>
@@ -3548,8 +3638,11 @@
       <c r="V32" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W32" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A33" s="5" t="s">
         <v>231</v>
       </c>
@@ -3612,8 +3705,11 @@
       <c r="V33" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="34" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W33" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A34" s="5" t="s">
         <v>232</v>
       </c>
@@ -3680,8 +3776,11 @@
       <c r="V34" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="35" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W34" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A35" s="5" t="s">
         <v>233</v>
       </c>
@@ -3742,8 +3841,11 @@
       <c r="V35" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W35" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A36" s="5" t="s">
         <v>234</v>
       </c>
@@ -3806,8 +3908,11 @@
       <c r="V36" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="37" spans="1:22" ht="275.5" x14ac:dyDescent="0.35">
+      <c r="W36" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" ht="275.5" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>235</v>
       </c>
@@ -3874,8 +3979,11 @@
       <c r="V37" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="38" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W37" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A38" s="5" t="s">
         <v>236</v>
       </c>
@@ -3924,20 +4032,23 @@
       </c>
       <c r="Q38" s="12"/>
       <c r="R38" s="13"/>
-      <c r="S38" s="16">
+      <c r="S38" s="15">
         <v>1</v>
       </c>
       <c r="T38" s="13" t="s">
         <v>314</v>
       </c>
-      <c r="U38" s="17" t="s">
-        <v>347</v>
+      <c r="U38" s="16" t="s">
+        <v>345</v>
       </c>
       <c r="V38" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W38" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>237</v>
       </c>
@@ -3989,7 +4100,7 @@
       <c r="S39" s="13">
         <v>2</v>
       </c>
-      <c r="T39" s="18" t="s">
+      <c r="T39" s="16" t="s">
         <v>339</v>
       </c>
       <c r="U39" s="13" t="s">
@@ -3998,8 +4109,11 @@
       <c r="V39" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="40" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W39" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>238</v>
       </c>
@@ -4066,8 +4180,11 @@
       <c r="V40" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="41" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W40" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A41" s="5" t="s">
         <v>239</v>
       </c>
@@ -4128,8 +4245,11 @@
       <c r="V41" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W41" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>240</v>
       </c>
@@ -4190,8 +4310,11 @@
       <c r="V42" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="43" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W42" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>241</v>
       </c>
@@ -4256,8 +4379,11 @@
       <c r="V43" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="44" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W43" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>242</v>
       </c>
@@ -4318,8 +4444,11 @@
       <c r="V44" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W44" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A45" s="5" t="s">
         <v>243</v>
       </c>
@@ -4380,8 +4509,11 @@
       <c r="V45" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="46" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W45" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>244</v>
       </c>
@@ -4448,8 +4580,11 @@
       <c r="V46" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="47" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W46" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>245</v>
       </c>
@@ -4512,8 +4647,11 @@
       <c r="V47" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="48" spans="1:22" ht="42" x14ac:dyDescent="0.35">
+      <c r="W47" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>246</v>
       </c>
@@ -4576,8 +4714,11 @@
       <c r="V48" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="49" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W48" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>247</v>
       </c>
@@ -4644,8 +4785,11 @@
       <c r="V49" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="50" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W49" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="50" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A50" s="5" t="s">
         <v>248</v>
       </c>
@@ -4708,8 +4852,11 @@
       <c r="V50" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="51" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W50" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A51" s="5" t="s">
         <v>249</v>
       </c>
@@ -4772,8 +4919,11 @@
       <c r="V51" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="52" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W51" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="52" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A52" s="5" t="s">
         <v>250</v>
       </c>
@@ -4840,8 +4990,11 @@
       <c r="V52" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="53" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W52" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>251</v>
       </c>
@@ -4904,8 +5057,11 @@
       <c r="V53" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="54" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W53" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="54" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
         <v>252</v>
       </c>
@@ -4968,8 +5124,11 @@
       <c r="V54" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="55" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W54" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="55" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>253</v>
       </c>
@@ -5036,8 +5195,11 @@
       <c r="V55" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="56" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W55" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="56" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>254</v>
       </c>
@@ -5100,8 +5262,11 @@
       <c r="V56" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="57" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W56" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>255</v>
       </c>
@@ -5164,8 +5329,11 @@
       <c r="V57" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="58" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W57" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="58" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>256</v>
       </c>
@@ -5232,8 +5400,11 @@
       <c r="V58" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="59" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W58" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>257</v>
       </c>
@@ -5296,8 +5467,11 @@
       <c r="V59" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="60" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W59" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>258</v>
       </c>
@@ -5358,8 +5532,11 @@
       <c r="V60" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="61" spans="1:22" ht="280" x14ac:dyDescent="0.35">
+      <c r="W60" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="280" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>259</v>
       </c>
@@ -5426,8 +5603,11 @@
       <c r="V61" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="62" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W61" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>260</v>
       </c>
@@ -5488,8 +5668,11 @@
       <c r="V62" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="63" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W62" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
         <v>261</v>
       </c>
@@ -5550,8 +5733,11 @@
       <c r="V63" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="64" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W63" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>262</v>
       </c>
@@ -5618,8 +5804,11 @@
       <c r="V64" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="65" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W64" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>263</v>
       </c>
@@ -5682,8 +5871,11 @@
       <c r="V65" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W65" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>264</v>
       </c>
@@ -5744,8 +5936,11 @@
       <c r="V66" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="67" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W66" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
         <v>265</v>
       </c>
@@ -5812,8 +6007,11 @@
       <c r="V67" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="68" spans="1:22" ht="42" x14ac:dyDescent="0.35">
+      <c r="W67" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" ht="42" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>266</v>
       </c>
@@ -5876,8 +6074,11 @@
       <c r="V68" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="69" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W68" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="69" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>267</v>
       </c>
@@ -5942,8 +6143,11 @@
       <c r="V69" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="70" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W69" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="70" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>268</v>
       </c>
@@ -6004,8 +6208,11 @@
       <c r="V70" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W70" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="71" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A71" s="5" t="s">
         <v>269</v>
       </c>
@@ -6066,8 +6273,11 @@
       <c r="V71" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W71" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="72" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>270</v>
       </c>
@@ -6104,8 +6314,11 @@
       <c r="V72" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W72" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="73" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>271</v>
       </c>
@@ -6168,8 +6381,11 @@
       <c r="V73" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="74" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W73" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A74" s="5" t="s">
         <v>272</v>
       </c>
@@ -6236,8 +6452,11 @@
       <c r="V74" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="75" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W74" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>273</v>
       </c>
@@ -6300,8 +6519,11 @@
       <c r="V75" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="76" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W75" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="76" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>274</v>
       </c>
@@ -6364,8 +6586,11 @@
       <c r="V76" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="77" spans="1:22" ht="56" x14ac:dyDescent="0.35">
+      <c r="W76" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="77" spans="1:23" ht="56" x14ac:dyDescent="0.35">
       <c r="A77" s="5" t="s">
         <v>275</v>
       </c>
@@ -6428,8 +6653,11 @@
       <c r="V77" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W77" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="78" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>276</v>
       </c>
@@ -6492,8 +6720,11 @@
       <c r="V78" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W78" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="79" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>277</v>
       </c>
@@ -6552,8 +6783,11 @@
       <c r="V79" s="7" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W79" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="80" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>278</v>
       </c>
@@ -6616,8 +6850,11 @@
       <c r="V80" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="81" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W80" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="81" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>279</v>
       </c>
@@ -6680,8 +6917,11 @@
       <c r="V81" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="82" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W81" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>280</v>
       </c>
@@ -6744,8 +6984,11 @@
       <c r="V82" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="83" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W82" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="83" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>281</v>
       </c>
@@ -6808,8 +7051,11 @@
       <c r="V83" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="84" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W83" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="84" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A84" s="5" t="s">
         <v>282</v>
       </c>
@@ -6872,8 +7118,11 @@
       <c r="V84" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="85" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="W84" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="85" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>283</v>
       </c>
@@ -6936,8 +7185,11 @@
       <c r="V85" s="13" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="86" spans="1:22" ht="28" x14ac:dyDescent="0.35">
+      <c r="W85" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="86" spans="1:23" ht="28" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>284</v>
       </c>
@@ -6999,6 +7251,9 @@
       </c>
       <c r="V86" s="13" t="s">
         <v>331</v>
+      </c>
+      <c r="W86" s="13">
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -7013,10 +7268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -7027,9 +7282,10 @@
     <col min="4" max="5" width="19" customWidth="1"/>
     <col min="6" max="6" width="40.54296875" customWidth="1"/>
     <col min="7" max="7" width="35.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -7051,8 +7307,11 @@
       <c r="G1" s="2" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
@@ -7068,8 +7327,11 @@
       <c r="G2" s="1" t="s">
         <v>61</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="H2" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="409.5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -7086,10 +7348,13 @@
         <v>333</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>67</v>
+      </c>
+      <c r="H3" s="13">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>